<commit_message>
Change prosumer output under new salvage
</commit_message>
<xml_diff>
--- a/Outputs/3. Prosumer percentage/Base Cases/10/Output_0_40.xlsx
+++ b/Outputs/3. Prosumer percentage/Base Cases/10/Output_0_40.xlsx
@@ -480,8 +480,10 @@
           <t>Required Level of Met Demand</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -501,7 +503,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2756962.499472995</v>
+        <v>2745209.194653912</v>
       </c>
     </row>
     <row r="7">
@@ -521,7 +523,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>547990.1264613952</v>
+        <v>613365.4189157155</v>
       </c>
     </row>
     <row r="9">
@@ -541,7 +543,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8142818.707058895</v>
+        <v>8128938.055953957</v>
       </c>
     </row>
     <row r="11">
@@ -23255,7 +23257,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>27.67496150217681</v>
+        <v>26.37807130498146</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -23264,16 +23266,16 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>23.07718884140098</v>
+        <v>21.78029864420563</v>
       </c>
       <c r="F11" t="n">
-        <v>62.26505147848269</v>
+        <v>60.96816128128734</v>
       </c>
       <c r="G11" t="n">
-        <v>86.7088554793757</v>
+        <v>85.41196528218035</v>
       </c>
       <c r="H11" t="n">
-        <v>27.21506248173574</v>
+        <v>25.91817228454039</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -23285,7 +23287,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>7.927015798719992</v>
+        <v>6.630125601524639</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -23297,7 +23299,7 @@
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>1.296890197195353</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
@@ -23321,10 +23323,10 @@
         <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>11.93551320862656</v>
+        <v>10.63862301143121</v>
       </c>
       <c r="Y11" t="n">
-        <v>41.04761030029579</v>
+        <v>39.75072010310043</v>
       </c>
     </row>
     <row r="12">
@@ -23729,7 +23731,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>15.73944829355025</v>
+        <v>19.74794570345682</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -23738,16 +23740,16 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>11.14167563277442</v>
+        <v>15.15017304268099</v>
       </c>
       <c r="F17" t="n">
-        <v>50.32953826985613</v>
+        <v>54.3380356797627</v>
       </c>
       <c r="G17" t="n">
-        <v>74.77334227074914</v>
+        <v>78.78183968065571</v>
       </c>
       <c r="H17" t="n">
-        <v>15.27954927310918</v>
+        <v>19.28804668301575</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -23795,10 +23797,10 @@
         <v>0</v>
       </c>
       <c r="X17" t="n">
-        <v>0</v>
+        <v>4.008497409906568</v>
       </c>
       <c r="Y17" t="n">
-        <v>29.11209709166923</v>
+        <v>33.12059450157579</v>
       </c>
     </row>
     <row r="18">
@@ -23966,7 +23968,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>15.73944829355025</v>
+        <v>19.74794570345682</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -23975,16 +23977,16 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>11.14167563277442</v>
+        <v>15.15017304268099</v>
       </c>
       <c r="F20" t="n">
-        <v>50.32953826985613</v>
+        <v>54.3380356797627</v>
       </c>
       <c r="G20" t="n">
-        <v>74.77334227074914</v>
+        <v>78.78183968065571</v>
       </c>
       <c r="H20" t="n">
-        <v>15.27954927310918</v>
+        <v>19.28804668301575</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -24032,10 +24034,10 @@
         <v>0</v>
       </c>
       <c r="X20" t="n">
-        <v>0</v>
+        <v>4.008497409906568</v>
       </c>
       <c r="Y20" t="n">
-        <v>29.11209709166923</v>
+        <v>33.12059450157579</v>
       </c>
     </row>
     <row r="21">
@@ -24203,7 +24205,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>15.73944829355025</v>
+        <v>19.74794570345682</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -24212,16 +24214,16 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>11.14167563277442</v>
+        <v>15.15017304268099</v>
       </c>
       <c r="F23" t="n">
-        <v>50.32953826985613</v>
+        <v>54.3380356797627</v>
       </c>
       <c r="G23" t="n">
-        <v>74.77334227074914</v>
+        <v>78.78183968065571</v>
       </c>
       <c r="H23" t="n">
-        <v>15.27954927310918</v>
+        <v>19.28804668301575</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -24269,10 +24271,10 @@
         <v>0</v>
       </c>
       <c r="X23" t="n">
-        <v>0</v>
+        <v>4.008497409906568</v>
       </c>
       <c r="Y23" t="n">
-        <v>29.11209709166923</v>
+        <v>33.12059450157579</v>
       </c>
     </row>
     <row r="24">
@@ -24440,7 +24442,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>27.67496150217681</v>
+        <v>26.37807130498146</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -24449,16 +24451,16 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>23.07718884140098</v>
+        <v>21.78029864420563</v>
       </c>
       <c r="F26" t="n">
-        <v>62.26505147848269</v>
+        <v>60.96816128128734</v>
       </c>
       <c r="G26" t="n">
-        <v>86.7088554793757</v>
+        <v>85.41196528218035</v>
       </c>
       <c r="H26" t="n">
-        <v>27.21506248173574</v>
+        <v>25.91817228454039</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -24470,7 +24472,7 @@
         <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>7.927015798719992</v>
+        <v>6.630125601524639</v>
       </c>
       <c r="M26" t="n">
         <v>0</v>
@@ -24482,7 +24484,7 @@
         <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>1.296890197195353</v>
+        <v>0</v>
       </c>
       <c r="Q26" t="n">
         <v>0</v>
@@ -24506,10 +24508,10 @@
         <v>0</v>
       </c>
       <c r="X26" t="n">
-        <v>11.93551320862656</v>
+        <v>10.63862301143121</v>
       </c>
       <c r="Y26" t="n">
-        <v>41.04761030029579</v>
+        <v>39.75072010310043</v>
       </c>
     </row>
     <row r="27">
@@ -24677,7 +24679,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>20.96594200063248</v>
+        <v>26.37807130498146</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -24686,16 +24688,16 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>16.36816933985665</v>
+        <v>21.78029864420563</v>
       </c>
       <c r="F29" t="n">
-        <v>55.55603197693836</v>
+        <v>60.96816128128734</v>
       </c>
       <c r="G29" t="n">
-        <v>79.99983597783137</v>
+        <v>85.41196528218035</v>
       </c>
       <c r="H29" t="n">
-        <v>20.50604298019141</v>
+        <v>25.91817228454039</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -24707,7 +24709,7 @@
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>1.217996297175659</v>
+        <v>6.630125601524639</v>
       </c>
       <c r="M29" t="n">
         <v>0</v>
@@ -24743,10 +24745,10 @@
         <v>0</v>
       </c>
       <c r="X29" t="n">
-        <v>5.226493707082227</v>
+        <v>10.63862301143121</v>
       </c>
       <c r="Y29" t="n">
-        <v>34.33859079875145</v>
+        <v>39.75072010310043</v>
       </c>
     </row>
     <row r="30">
@@ -24914,7 +24916,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.4598990204410711</v>
+        <v>19.74794570345682</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -24923,16 +24925,16 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>15.15017304268099</v>
       </c>
       <c r="F32" t="n">
-        <v>35.04998899674695</v>
+        <v>54.3380356797627</v>
       </c>
       <c r="G32" t="n">
-        <v>59.49379299763996</v>
+        <v>78.78183968065571</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>19.28804668301575</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -24980,10 +24982,10 @@
         <v>0</v>
       </c>
       <c r="X32" t="n">
-        <v>0</v>
+        <v>4.008497409906568</v>
       </c>
       <c r="Y32" t="n">
-        <v>13.83254781856004</v>
+        <v>33.12059450157579</v>
       </c>
     </row>
     <row r="33">
@@ -25151,7 +25153,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.4598990204410711</v>
+        <v>19.74794570345682</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -25160,16 +25162,16 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>15.15017304268099</v>
       </c>
       <c r="F35" t="n">
-        <v>35.04998899674695</v>
+        <v>54.3380356797627</v>
       </c>
       <c r="G35" t="n">
-        <v>59.49379299763996</v>
+        <v>78.78183968065571</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>19.28804668301575</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -25217,10 +25219,10 @@
         <v>0</v>
       </c>
       <c r="X35" t="n">
-        <v>0</v>
+        <v>4.008497409906568</v>
       </c>
       <c r="Y35" t="n">
-        <v>13.83254781856004</v>
+        <v>33.12059450157579</v>
       </c>
     </row>
     <row r="36">
@@ -25388,7 +25390,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.4598990204410711</v>
+        <v>19.74794570345682</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -25397,16 +25399,16 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>15.15017304268099</v>
       </c>
       <c r="F38" t="n">
-        <v>35.04998899674695</v>
+        <v>54.3380356797627</v>
       </c>
       <c r="G38" t="n">
-        <v>59.49379299763996</v>
+        <v>78.78183968065571</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>19.28804668301575</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -25454,10 +25456,10 @@
         <v>0</v>
       </c>
       <c r="X38" t="n">
-        <v>0</v>
+        <v>4.008497409906568</v>
       </c>
       <c r="Y38" t="n">
-        <v>13.83254781856004</v>
+        <v>33.12059450157579</v>
       </c>
     </row>
     <row r="39">
@@ -25625,7 +25627,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>27.67496150217681</v>
+        <v>26.37807130498146</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -25634,16 +25636,16 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>23.07718884140098</v>
+        <v>21.78029864420563</v>
       </c>
       <c r="F41" t="n">
-        <v>62.26505147848269</v>
+        <v>60.96816128128734</v>
       </c>
       <c r="G41" t="n">
-        <v>86.7088554793757</v>
+        <v>85.41196528218035</v>
       </c>
       <c r="H41" t="n">
-        <v>27.21506248173574</v>
+        <v>25.91817228454039</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -25655,7 +25657,7 @@
         <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>7.927015798719992</v>
+        <v>6.630125601524639</v>
       </c>
       <c r="M41" t="n">
         <v>0</v>
@@ -25667,7 +25669,7 @@
         <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>1.296890197195353</v>
+        <v>0</v>
       </c>
       <c r="Q41" t="n">
         <v>0</v>
@@ -25691,10 +25693,10 @@
         <v>0</v>
       </c>
       <c r="X41" t="n">
-        <v>11.93551320862656</v>
+        <v>10.63862301143121</v>
       </c>
       <c r="Y41" t="n">
-        <v>41.04761030029579</v>
+        <v>39.75072010310043</v>
       </c>
     </row>
     <row r="42">
@@ -25862,25 +25864,25 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>35.6808712009165</v>
+        <v>26.37807130498146</v>
       </c>
       <c r="C44" t="n">
-        <v>4.721663078061795</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>31.08309854014067</v>
+        <v>21.78029864420563</v>
       </c>
       <c r="F44" t="n">
-        <v>70.27096117722238</v>
+        <v>60.96816128128734</v>
       </c>
       <c r="G44" t="n">
-        <v>94.71476517811539</v>
+        <v>85.41196528218035</v>
       </c>
       <c r="H44" t="n">
-        <v>35.22097218047543</v>
+        <v>25.91817228454039</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -25892,19 +25894,19 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>15.93292549745968</v>
+        <v>6.630125601524639</v>
       </c>
       <c r="M44" t="n">
-        <v>8.005909698739686</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>6.641149113867584</v>
+        <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>7.64317780807022</v>
+        <v>0</v>
       </c>
       <c r="P44" t="n">
-        <v>9.302799895935038</v>
+        <v>0</v>
       </c>
       <c r="Q44" t="n">
         <v>0</v>
@@ -25928,10 +25930,10 @@
         <v>0</v>
       </c>
       <c r="X44" t="n">
-        <v>19.94142290736625</v>
+        <v>10.63862301143121</v>
       </c>
       <c r="Y44" t="n">
-        <v>49.05351999903547</v>
+        <v>39.75072010310043</v>
       </c>
     </row>
     <row r="45">
@@ -26147,7 +26149,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>697341.9452204062</v>
+        <v>698038.7643233592</v>
       </c>
     </row>
     <row r="6">
@@ -26163,7 +26165,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>702880.4633782475</v>
+        <v>701205.3123106475</v>
       </c>
     </row>
     <row r="8">
@@ -26171,7 +26173,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>702880.4633782475</v>
+        <v>701205.3123106475</v>
       </c>
     </row>
     <row r="9">
@@ -26179,7 +26181,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>702880.4633782475</v>
+        <v>701205.3123106475</v>
       </c>
     </row>
     <row r="10">
@@ -26187,7 +26189,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>697341.9452204062</v>
+        <v>698038.7643233592</v>
       </c>
     </row>
     <row r="11">
@@ -26195,7 +26197,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>700623.5972791164</v>
+        <v>698038.7643233592</v>
       </c>
     </row>
     <row r="12">
@@ -26203,7 +26205,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>708106.5668715471</v>
+        <v>701205.3123106475</v>
       </c>
     </row>
     <row r="13">
@@ -26211,7 +26213,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>708106.5668715471</v>
+        <v>701205.3123106475</v>
       </c>
     </row>
     <row r="14">
@@ -26219,7 +26221,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>708106.5668715471</v>
+        <v>701205.3123106475</v>
       </c>
     </row>
     <row r="15">
@@ -26227,7 +26229,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>697341.9452204062</v>
+        <v>698038.7643233592</v>
       </c>
     </row>
     <row r="16">
@@ -26235,7 +26237,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>691427.7595272586</v>
+        <v>698038.7643233592</v>
       </c>
     </row>
   </sheetData>
@@ -26320,40 +26322,40 @@
         <v>950927.6713398893</v>
       </c>
       <c r="E2" t="n">
-        <v>929789.260293875</v>
+        <v>930718.3524311456</v>
       </c>
       <c r="F2" t="n">
         <v>930718.3524311456</v>
       </c>
       <c r="G2" t="n">
-        <v>937173.9511709965</v>
+        <v>934940.4164141967</v>
       </c>
       <c r="H2" t="n">
-        <v>937173.9511709965</v>
+        <v>934940.4164141967</v>
       </c>
       <c r="I2" t="n">
-        <v>937173.9511709965</v>
+        <v>934940.4164141967</v>
       </c>
       <c r="J2" t="n">
-        <v>929789.260293875</v>
+        <v>930718.3524311456</v>
       </c>
       <c r="K2" t="n">
-        <v>934164.7963721551</v>
+        <v>930718.3524311456</v>
       </c>
       <c r="L2" t="n">
-        <v>944142.0891620629</v>
+        <v>934940.4164141967</v>
       </c>
       <c r="M2" t="n">
-        <v>944142.0891620629</v>
+        <v>934940.4164141967</v>
       </c>
       <c r="N2" t="n">
-        <v>944142.0891620629</v>
+        <v>934940.4164141967</v>
       </c>
       <c r="O2" t="n">
-        <v>929789.260293875</v>
+        <v>930718.3524311456</v>
       </c>
       <c r="P2" t="n">
-        <v>921903.6793696781</v>
+        <v>930718.3524311456</v>
       </c>
     </row>
     <row r="3">
@@ -26372,13 +26374,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>269505.0928759091</v>
+        <v>270542.6050336653</v>
       </c>
       <c r="F3" t="n">
-        <v>1037.512157756282</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>8510.898409144966</v>
+        <v>5304.100481219757</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -26387,13 +26389,13 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>259956.6823090078</v>
+        <v>265238.5045524456</v>
       </c>
       <c r="K3" t="n">
-        <v>6404.727758991748</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>24915.73279329809</v>
+        <v>10608.20096243947</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -26402,7 +26404,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>238184.6323236192</v>
+        <v>259934.4040712259</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -26424,40 +26426,40 @@
         <v>542758.2060475298</v>
       </c>
       <c r="E4" t="n">
-        <v>530693.0969926381</v>
+        <v>531223.3921947614</v>
       </c>
       <c r="F4" t="n">
         <v>531223.3921947614</v>
       </c>
       <c r="G4" t="n">
-        <v>534908.0354085478</v>
+        <v>533633.2073072293</v>
       </c>
       <c r="H4" t="n">
-        <v>534908.0354085478</v>
+        <v>533633.2073072293</v>
       </c>
       <c r="I4" t="n">
-        <v>534908.0354085478</v>
+        <v>533633.2073072293</v>
       </c>
       <c r="J4" t="n">
-        <v>530693.0969926381</v>
+        <v>531223.3921947614</v>
       </c>
       <c r="K4" t="n">
-        <v>533190.5089240812</v>
+        <v>531223.3921947614</v>
       </c>
       <c r="L4" t="n">
-        <v>538885.2191518643</v>
+        <v>533633.2073072293</v>
       </c>
       <c r="M4" t="n">
-        <v>538885.2191518643</v>
+        <v>533633.2073072293</v>
       </c>
       <c r="N4" t="n">
-        <v>538885.2191518643</v>
+        <v>533633.2073072293</v>
       </c>
       <c r="O4" t="n">
-        <v>530693.0969926381</v>
+        <v>531223.3921947614</v>
       </c>
       <c r="P4" t="n">
-        <v>526192.2670293781</v>
+        <v>531223.3921947614</v>
       </c>
     </row>
     <row r="5">
@@ -26476,40 +26478,40 @@
         <v>33627.6</v>
       </c>
       <c r="E5" t="n">
-        <v>28321.279566231</v>
+        <v>28430.30782821902</v>
       </c>
       <c r="F5" t="n">
         <v>28430.30782821902</v>
       </c>
       <c r="G5" t="n">
-        <v>29324.68622616703</v>
+        <v>28987.69585741359</v>
       </c>
       <c r="H5" t="n">
-        <v>29324.68622616703</v>
+        <v>28987.69585741359</v>
       </c>
       <c r="I5" t="n">
-        <v>29324.68622616703</v>
+        <v>28987.69585741359</v>
       </c>
       <c r="J5" t="n">
-        <v>28321.279566231</v>
+        <v>28430.30782821902</v>
       </c>
       <c r="K5" t="n">
-        <v>28885.30012670633</v>
+        <v>28430.30782821902</v>
       </c>
       <c r="L5" t="n">
-        <v>30609.22265400804</v>
+        <v>28987.69585741359</v>
       </c>
       <c r="M5" t="n">
-        <v>30609.22265400804</v>
+        <v>28987.69585741359</v>
       </c>
       <c r="N5" t="n">
-        <v>30609.22265400804</v>
+        <v>28987.69585741359</v>
       </c>
       <c r="O5" t="n">
-        <v>28321.279566231</v>
+        <v>28430.30782821902</v>
       </c>
       <c r="P5" t="n">
-        <v>27648.23074376765</v>
+        <v>28430.30782821902</v>
       </c>
     </row>
     <row r="6">
@@ -26528,40 +26530,40 @@
         <v>374541.8652923595</v>
       </c>
       <c r="E6" t="n">
-        <v>101269.7908590969</v>
+        <v>100522.0473744998</v>
       </c>
       <c r="F6" t="n">
-        <v>370027.1402504089</v>
+        <v>371064.6524081652</v>
       </c>
       <c r="G6" t="n">
-        <v>364430.3311271367</v>
+        <v>367015.4127683342</v>
       </c>
       <c r="H6" t="n">
-        <v>372941.2295362817</v>
+        <v>372319.5132495539</v>
       </c>
       <c r="I6" t="n">
-        <v>372941.2295362817</v>
+        <v>372319.5132495539</v>
       </c>
       <c r="J6" t="n">
-        <v>110818.2014259981</v>
+        <v>105826.1478557196</v>
       </c>
       <c r="K6" t="n">
-        <v>365684.2595623758</v>
+        <v>371064.6524081652</v>
       </c>
       <c r="L6" t="n">
-        <v>349731.9145628924</v>
+        <v>361711.3122871144</v>
       </c>
       <c r="M6" t="n">
-        <v>374647.6473561905</v>
+        <v>372319.5132495539</v>
       </c>
       <c r="N6" t="n">
-        <v>374647.6473561905</v>
+        <v>372319.5132495539</v>
       </c>
       <c r="O6" t="n">
-        <v>132590.2514113868</v>
+        <v>111130.2483369393</v>
       </c>
       <c r="P6" t="n">
-        <v>368063.1815965324</v>
+        <v>371064.6524081652</v>
       </c>
     </row>
   </sheetData>
@@ -26692,40 +26694,40 @@
         <v>400</v>
       </c>
       <c r="E2" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="F2" t="n">
         <v>338.1782562920817</v>
       </c>
       <c r="G2" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="H2" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="I2" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="J2" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="K2" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="L2" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="M2" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="N2" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="O2" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="P2" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
     </row>
     <row r="3">
@@ -26914,13 +26916,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920816</v>
       </c>
       <c r="F2" t="n">
-        <v>1.296890197195353</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>10.63862301143121</v>
+        <v>6.630125601524696</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -26929,13 +26931,13 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>324.9458528862597</v>
+        <v>331.548130690557</v>
       </c>
       <c r="K2" t="n">
-        <v>8.005909698739686</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>31.14466599162262</v>
+        <v>13.26025120304934</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -26944,7 +26946,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>297.730790404524</v>
+        <v>324.9180050890324</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -27151,13 +27153,13 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920816</v>
       </c>
       <c r="K2" t="n">
-        <v>1.296890197195353</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>10.63862301143121</v>
+        <v>6.630125601524696</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -27166,10 +27168,10 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>324.9458528862597</v>
+        <v>331.548130690557</v>
       </c>
       <c r="P2" t="n">
-        <v>8.005909698739686</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -28087,7 +28089,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="C11" t="n">
         <v>333.5971194742085</v>
@@ -28096,16 +28098,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="F11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="G11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="H11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="I11" t="n">
         <v>307.6301510626203</v>
@@ -28117,7 +28119,7 @@
         <v>321.881407153284</v>
       </c>
       <c r="L11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="M11" t="n">
         <v>336.8813660948863</v>
@@ -28129,7 +28131,7 @@
         <v>336.5186342042169</v>
       </c>
       <c r="P11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Q11" t="n">
         <v>325.1220714413824</v>
@@ -28153,10 +28155,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Y11" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
     </row>
     <row r="12">
@@ -28561,7 +28563,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="C17" t="n">
         <v>333.5971194742085</v>
@@ -28570,16 +28572,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E17" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="F17" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="G17" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="H17" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="I17" t="n">
         <v>307.6301510626203</v>
@@ -28627,10 +28629,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X17" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="Y17" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
     </row>
     <row r="18">
@@ -28798,7 +28800,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="C20" t="n">
         <v>333.5971194742085</v>
@@ -28807,16 +28809,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E20" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="F20" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="G20" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="H20" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="I20" t="n">
         <v>307.6301510626203</v>
@@ -28864,10 +28866,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X20" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="Y20" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
     </row>
     <row r="21">
@@ -29035,7 +29037,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="C23" t="n">
         <v>333.5971194742085</v>
@@ -29044,16 +29046,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E23" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="F23" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="G23" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="H23" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="I23" t="n">
         <v>307.6301510626203</v>
@@ -29101,10 +29103,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X23" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="Y23" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
     </row>
     <row r="24">
@@ -29272,7 +29274,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="C26" t="n">
         <v>333.5971194742085</v>
@@ -29281,16 +29283,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="F26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="G26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="H26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="I26" t="n">
         <v>307.6301510626203</v>
@@ -29302,7 +29304,7 @@
         <v>321.881407153284</v>
       </c>
       <c r="L26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="M26" t="n">
         <v>336.8813660948863</v>
@@ -29314,7 +29316,7 @@
         <v>336.5186342042169</v>
       </c>
       <c r="P26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Q26" t="n">
         <v>325.1220714413824</v>
@@ -29338,10 +29340,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Y26" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
     </row>
     <row r="27">
@@ -29509,7 +29511,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="C29" t="n">
         <v>333.5971194742085</v>
@@ -29518,16 +29520,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E29" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="F29" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="G29" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="H29" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="I29" t="n">
         <v>307.6301510626203</v>
@@ -29539,7 +29541,7 @@
         <v>321.881407153284</v>
       </c>
       <c r="L29" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="M29" t="n">
         <v>336.8813660948863</v>
@@ -29575,10 +29577,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X29" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Y29" t="n">
-        <v>343.5903855964307</v>
+        <v>338.1782562920817</v>
       </c>
     </row>
     <row r="30">
@@ -29746,7 +29748,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="C32" t="n">
         <v>333.5971194742085</v>
@@ -29755,16 +29757,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E32" t="n">
-        <v>359.9585549362873</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="F32" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="G32" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="H32" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="I32" t="n">
         <v>307.6301510626203</v>
@@ -29812,10 +29814,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X32" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="Y32" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
     </row>
     <row r="33">
@@ -29983,7 +29985,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="C35" t="n">
         <v>333.5971194742085</v>
@@ -29992,16 +29994,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E35" t="n">
-        <v>359.9585549362873</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="F35" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="G35" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="H35" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="I35" t="n">
         <v>307.6301510626203</v>
@@ -30049,10 +30051,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X35" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="Y35" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
     </row>
     <row r="36">
@@ -30220,7 +30222,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="C38" t="n">
         <v>333.5971194742085</v>
@@ -30229,16 +30231,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E38" t="n">
-        <v>359.9585549362873</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="F38" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="G38" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="H38" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="I38" t="n">
         <v>307.6301510626203</v>
@@ -30286,10 +30288,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X38" t="n">
-        <v>348.8168793035129</v>
+        <v>344.8083818936063</v>
       </c>
       <c r="Y38" t="n">
-        <v>364.0964285766221</v>
+        <v>344.8083818936063</v>
       </c>
     </row>
     <row r="39">
@@ -30457,7 +30459,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="C41" t="n">
         <v>333.5971194742085</v>
@@ -30466,16 +30468,16 @@
         <v>319.1317556432476</v>
       </c>
       <c r="E41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="F41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="G41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="H41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="I41" t="n">
         <v>307.6301510626203</v>
@@ -30487,7 +30489,7 @@
         <v>321.881407153284</v>
       </c>
       <c r="L41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="M41" t="n">
         <v>336.8813660948863</v>
@@ -30499,7 +30501,7 @@
         <v>336.5186342042169</v>
       </c>
       <c r="P41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Q41" t="n">
         <v>325.1220714413824</v>
@@ -30523,10 +30525,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Y41" t="n">
-        <v>336.8813660948863</v>
+        <v>338.1782562920817</v>
       </c>
     </row>
     <row r="42">
@@ -30694,25 +30696,25 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="C44" t="n">
-        <v>328.8754563961467</v>
+        <v>333.5971194742085</v>
       </c>
       <c r="D44" t="n">
         <v>319.1317556432476</v>
       </c>
       <c r="E44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="F44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="G44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="H44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="I44" t="n">
         <v>307.6301510626203</v>
@@ -30724,19 +30726,19 @@
         <v>321.881407153284</v>
       </c>
       <c r="L44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="M44" t="n">
-        <v>328.8754563961467</v>
+        <v>336.8813660948863</v>
       </c>
       <c r="N44" t="n">
-        <v>328.8754563961467</v>
+        <v>335.5166055100142</v>
       </c>
       <c r="O44" t="n">
-        <v>328.8754563961467</v>
+        <v>336.5186342042169</v>
       </c>
       <c r="P44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Q44" t="n">
         <v>325.1220714413824</v>
@@ -30760,10 +30762,10 @@
         <v>325.3917254792934</v>
       </c>
       <c r="X44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
       <c r="Y44" t="n">
-        <v>328.8754563961467</v>
+        <v>338.1782562920817</v>
       </c>
     </row>
     <row r="45">

</xml_diff>